<commit_message>
Ran 2023-08-27 Autopsy stats
</commit_message>
<xml_diff>
--- a/output/2022-11_autopsy-counts.xlsx
+++ b/output/2022-11_autopsy-counts.xlsx
@@ -8095,8 +8095,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010055E7AF632A704D4CBB1BD9FA14B19970" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5705bc62546c00eb30d3e393ea3d800">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" xmlns:ns3="852f286e-3e14-48be-b416-81218d12f978" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c29e53287aa3a112937d5a643cee4298" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010055E7AF632A704D4CBB1BD9FA14B19970" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a142d422042ab65c5cf1bdc7db96e15">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" xmlns:ns3="852f286e-3e14-48be-b416-81218d12f978" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c40a8bb7e01840c9a3629736cac3e4c1" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="edae88a8-d9dc-4074-a55b-fb97cb2cd74d"/>
     <xsd:import namespace="852f286e-3e14-48be-b416-81218d12f978"/>
@@ -8122,6 +8122,7 @@
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -8206,6 +8207,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="25" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="852f286e-3e14-48be-b416-81218d12f978" elementFormDefault="qualified">
@@ -8371,7 +8377,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC0B31F0-4E96-41D0-B5C6-DA06F9C72D9B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3981C84-4C37-4726-BE02-D6FBA27161E1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>